<commit_message>
Agregar métricas de GB y HW
</commit_message>
<xml_diff>
--- a/Results/Resultados.xlsx
+++ b/Results/Resultados.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
-  <si>
-    <t>model_type</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>model_name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>Tipo de Modelo</t>
+  </si>
+  <si>
+    <t>Modelo</t>
   </si>
   <si>
     <t>rmse_train</t>
@@ -46,12 +43,15 @@
     <t>Estadístico Tradicional</t>
   </si>
   <si>
+    <t>Holt-Winters</t>
+  </si>
+  <si>
+    <t>Holt-Winters Log</t>
+  </si>
+  <si>
     <t>Regresión OLS</t>
   </si>
   <si>
-    <t>RegressionResultsWrapper</t>
-  </si>
-  <si>
     <t>Regresión OLS_Log</t>
   </si>
   <si>
@@ -64,9 +64,6 @@
     <t>SARIMAX Train Once - Test Once</t>
   </si>
   <si>
-    <t>SARIMAX</t>
-  </si>
-  <si>
     <t>SARIMAX log Train Once Test Once</t>
   </si>
   <si>
@@ -79,19 +76,19 @@
     <t>Machine Learning</t>
   </si>
   <si>
+    <t>Gradient Boosting</t>
+  </si>
+  <si>
+    <t>Gradient Boosting Log</t>
+  </si>
+  <si>
     <t>Random Forest</t>
   </si>
   <si>
-    <t>RandomForestRegressor</t>
-  </si>
-  <si>
     <t>Random Forest Log</t>
   </si>
   <si>
     <t>XGBoost</t>
-  </si>
-  <si>
-    <t>XGBRegressor</t>
   </si>
   <si>
     <t>XGBoost Log</t>
@@ -101,8 +98,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0_);($#,##0)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +110,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -123,15 +130,25 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFc3d69b"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95b3d7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -154,39 +171,56 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,401 +524,441 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="7.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="7.147857142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="7">
+        <v>21875.94</v>
+      </c>
+      <c r="D2" s="7">
+        <v>16132.76</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="F2" s="7">
+        <v>34673.32</v>
+      </c>
+      <c r="G2" s="7">
+        <v>25706.72</v>
+      </c>
+      <c r="H2" s="8">
+        <v>-0.77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="7">
+        <v>26988.45057462869</v>
+      </c>
+      <c r="D3" s="7">
+        <v>17946.32340906008</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.066928033834722</v>
+      </c>
+      <c r="F3" s="7">
+        <v>39001.46711238931</v>
+      </c>
+      <c r="G3" s="7">
+        <v>29369.89454680356</v>
+      </c>
+      <c r="H3" s="8">
+        <v>-1.234458174357315</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4">
+      <c r="C4" s="7">
         <v>21230.33</v>
       </c>
-      <c r="E2" s="4">
+      <c r="D4" s="7">
         <v>15806.68</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E4" s="8">
         <v>0.42</v>
       </c>
-      <c r="G2" s="4">
+      <c r="F4" s="7">
         <v>22236.82</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G4" s="7">
         <v>14988.69</v>
       </c>
-      <c r="I2" s="4">
+      <c r="H4" s="8">
         <v>0.27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C5" s="7">
         <v>23275.31</v>
       </c>
-      <c r="E3" s="4">
+      <c r="D5" s="7">
         <v>15265.18</v>
       </c>
-      <c r="F3" s="4">
+      <c r="E5" s="8">
         <v>0.31</v>
       </c>
-      <c r="G3" s="4">
+      <c r="F5" s="7">
         <v>34403.44</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G5" s="7">
         <v>25096.46</v>
       </c>
-      <c r="I3" s="4">
+      <c r="H5" s="8">
         <v>-0.74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C6" s="7">
         <v>21373.45</v>
       </c>
-      <c r="E4" s="5">
+      <c r="D6" s="7">
         <v>15363</v>
       </c>
-      <c r="F4" s="4">
+      <c r="E6" s="8">
         <v>0.41</v>
       </c>
-      <c r="G4" s="4">
+      <c r="F6" s="7">
         <v>22839.88</v>
       </c>
-      <c r="H4" s="4">
+      <c r="G6" s="7">
         <v>15387.59</v>
       </c>
-      <c r="I4" s="4">
+      <c r="H6" s="8">
         <v>0.23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C7" s="7">
         <v>22141.72</v>
       </c>
-      <c r="E5" s="4">
+      <c r="D7" s="9">
         <v>14721.3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="E7" s="8">
         <v>0.37</v>
       </c>
-      <c r="G5" s="4">
+      <c r="F7" s="7">
         <v>29015.48</v>
       </c>
-      <c r="H5" s="4">
+      <c r="G7" s="7">
         <v>20172.02</v>
       </c>
-      <c r="I5" s="4">
+      <c r="H7" s="8">
         <v>-0.24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C8" s="9">
+        <v>20704.87839449261</v>
+      </c>
+      <c r="D8" s="7">
+        <v>15358.54069813469</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.4508327809807866</v>
+      </c>
+      <c r="F8" s="9">
+        <v>19801.85914487888</v>
+      </c>
+      <c r="G8" s="9">
+        <v>14742.08705701988</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.4240002759034128</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="46.5" customFormat="1" s="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4">
+      <c r="C9" s="7">
+        <v>27199.61471925769</v>
+      </c>
+      <c r="D9" s="7">
+        <v>17453.11090356209</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.0522697522534588</v>
+      </c>
+      <c r="F9" s="7">
+        <v>26493.53840812254</v>
+      </c>
+      <c r="G9" s="7">
+        <v>17565.06577356985</v>
+      </c>
+      <c r="H9" s="8">
+        <v>-0.0310750367362222</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="9">
         <v>20704.87839449261</v>
       </c>
-      <c r="E6" s="4">
+      <c r="D10" s="7">
         <v>15358.54069813469</v>
       </c>
-      <c r="F6" s="4">
+      <c r="E10" s="10">
         <v>0.4508327809807866</v>
       </c>
-      <c r="G6" s="4">
-        <v>19801.85914487888</v>
-      </c>
-      <c r="H6" s="4">
-        <v>14742.08705701988</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0.4240002759034128</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="F10" s="7">
+        <v>20164.93180813319</v>
+      </c>
+      <c r="G10" s="7">
+        <v>15050.16851998996</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.4026844005828757</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7">
         <v>27199.61471925769</v>
       </c>
-      <c r="E7" s="4">
+      <c r="D11" s="7">
         <v>17453.11090356209</v>
       </c>
-      <c r="F7" s="4">
+      <c r="E11" s="8">
         <v>0.0522697522534588</v>
       </c>
-      <c r="G7" s="4">
-        <v>26493.53840812254</v>
-      </c>
-      <c r="H7" s="4">
-        <v>17565.06577356985</v>
-      </c>
-      <c r="I7" s="4">
-        <v>-0.0310750367362222</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4">
-        <v>20704.87839449261</v>
-      </c>
-      <c r="E8" s="4">
-        <v>15358.54069813469</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.4508327809807866</v>
-      </c>
-      <c r="G8" s="4">
-        <v>20164.93180813319</v>
-      </c>
-      <c r="H8" s="4">
-        <v>15050.16851998996</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0.4026844005828757</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="F11" s="7">
+        <v>26552.67851905519</v>
+      </c>
+      <c r="G11" s="7">
+        <v>17739.65292548016</v>
+      </c>
+      <c r="H11" s="8">
+        <v>-0.0356834019880101</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4">
-        <v>27199.61471925769</v>
-      </c>
-      <c r="E9" s="4">
-        <v>17453.11090356209</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.0522697522534588</v>
-      </c>
-      <c r="G9" s="4">
-        <v>26552.67851905519</v>
-      </c>
-      <c r="H9" s="4">
-        <v>17739.65292548016</v>
-      </c>
-      <c r="I9" s="4">
-        <v>-0.0356834019880101</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C12" s="7">
+        <v>15179.76</v>
+      </c>
+      <c r="D12" s="7">
+        <v>11154.27</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="F12" s="11">
+        <v>17795.4</v>
+      </c>
+      <c r="G12" s="7">
+        <v>12744.61</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C13" s="7">
+        <v>17926.74082054563</v>
+      </c>
+      <c r="D13" s="7">
+        <v>11108.03951158247</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.5883179642969272</v>
+      </c>
+      <c r="F13" s="7">
+        <v>18735.85975659958</v>
+      </c>
+      <c r="G13" s="7">
+        <v>12775.63109880941</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.4843469447036601</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4">
+      <c r="C14" s="7">
         <v>12982.65</v>
       </c>
-      <c r="E10" s="4">
+      <c r="D14" s="7">
         <v>9312.88</v>
       </c>
-      <c r="F10" s="4">
+      <c r="E14" s="8">
         <v>0.78</v>
       </c>
-      <c r="G10" s="5">
+      <c r="F14" s="7">
         <v>18095</v>
       </c>
-      <c r="H10" s="4">
+      <c r="G14" s="7">
         <v>12965.15</v>
       </c>
-      <c r="I10" s="4">
+      <c r="H14" s="8">
         <v>0.52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C15" s="11">
         <v>12031.71599534465</v>
       </c>
-      <c r="E11" s="4">
+      <c r="D15" s="11">
         <v>6681.630514850753</v>
       </c>
-      <c r="F11" s="4">
+      <c r="E15" s="12">
         <v>0.8145553190493142</v>
       </c>
-      <c r="G11" s="4">
+      <c r="F15" s="7">
         <v>20360.28767468741</v>
       </c>
-      <c r="H11" s="4">
+      <c r="G15" s="7">
         <v>13557.83308666786</v>
       </c>
-      <c r="I11" s="4">
+      <c r="H15" s="8">
         <v>0.391054870276276</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C16" s="7">
+        <v>15510.8</v>
+      </c>
+      <c r="D16" s="7">
+        <v>11218.9</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.69</v>
+      </c>
+      <c r="F16" s="7">
+        <v>17866.77</v>
+      </c>
+      <c r="G16" s="11">
+        <v>12555.63</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4">
-        <v>15510.8</v>
-      </c>
-      <c r="E12" s="4">
-        <v>11218.9</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0.69</v>
-      </c>
-      <c r="G12" s="4">
-        <v>17866.77</v>
-      </c>
-      <c r="H12" s="4">
-        <v>12555.63</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C17" s="7">
         <v>17333.41789522512</v>
       </c>
-      <c r="E13" s="4">
+      <c r="D17" s="7">
         <v>10682.38045538671</v>
       </c>
-      <c r="F13" s="4">
+      <c r="E17" s="8">
         <v>0.6151179541307276</v>
       </c>
-      <c r="G13" s="4">
+      <c r="F17" s="7">
         <v>19141.9021905896</v>
       </c>
-      <c r="H13" s="4">
+      <c r="G17" s="7">
         <v>13257.55491177267</v>
       </c>
-      <c r="I13" s="4">
+      <c r="H17" s="8">
         <v>0.4617543519352876</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>